<commit_message>
generation function examples added
</commit_message>
<xml_diff>
--- a/sample_apps/lab_app_en/lab_app_en_knowledge.xlsx
+++ b/sample_apps/lab_app_en/lab_app_en_knowledge.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nakano\system\dialbb\dialbb-v0.7\sample_apps\lab_app_en\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nakano\system\dialbb\dialbb-next\sample_apps\lab_app_en\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF736789-EAF2-436B-A907-D697056CFED9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D46CFC5-2D81-4FA6-B1D4-EE6FF8A792AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{C3566FB2-A815-41D8-9347-99D11DD601B4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{C3566FB2-A815-41D8-9347-99D11DD601B4}"/>
   </bookViews>
   <sheets>
     <sheet name="scenario" sheetId="1" r:id="rId1"/>
@@ -429,10 +429,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>{greeting}. I'm a ChatBot. If you don't mind, could you tell me your name?</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>#final_abort</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -446,6 +442,10 @@
   </si>
   <si>
     <t>_ne(#NE_PERSON, "")</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>{greeting}. I'm {get_system_name()}. If you don't mind, could you tell me your name?</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -630,9 +630,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office テーマ">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 テーマ">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -670,7 +670,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -776,7 +776,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -918,7 +918,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -929,7 +929,7 @@
   <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -985,7 +985,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="10" customFormat="1" ht="37.5" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:8" s="10" customFormat="1" ht="56.25" x14ac:dyDescent="0.4">
       <c r="A3" s="10" t="s">
         <v>29</v>
       </c>
@@ -993,16 +993,16 @@
         <v>43</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>82</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H3" s="10" t="s">
         <v>83</v>
@@ -1381,10 +1381,10 @@
         <v>29</v>
       </c>
       <c r="B25" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="C25" s="10" t="s">
         <v>102</v>
-      </c>
-      <c r="C25" s="10" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="26" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
syntax sugars in scenario descriptions
</commit_message>
<xml_diff>
--- a/sample_apps/lab_app_en/lab_app_en_knowledge.xlsx
+++ b/sample_apps/lab_app_en/lab_app_en_knowledge.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nakano\system\dialbb\dialbb-next\sample_apps\lab_app_en\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89FC8016-BBCE-4E57-8CF1-1AC09D612C08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B134791A-C885-4F52-9F49-8F5969BCE7C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{C3566FB2-A815-41D8-9347-99D11DD601B4}"/>
   </bookViews>
@@ -288,15 +288,9 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>_eq(#favorite-sandwich, "egg salad sandwich")</t>
-  </si>
-  <si>
     <t>is_known_sandwich(#favorite-sandwich)</t>
   </si>
   <si>
-    <t>_set(&amp;topic_sandwich,#favorite-sandwich)</t>
-  </si>
-  <si>
     <t>egg-salad-sandwich</t>
   </si>
   <si>
@@ -347,10 +341,6 @@
     <t>decide_greeting(&amp;greeting)</t>
   </si>
   <si>
-    <t>_set(&amp;topic_sandwich, #favorite-sandwich)</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>John.</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -375,14 +365,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>_eq(*confirmed, "yes")</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>_eq(*confirmed, "no")</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>{confirmation_request}</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -449,15 +431,35 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>_check_with_chatgpt("Please determine if the user said the reason.")</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>I'm sorry I couldn't understand. Thank you for your time.</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>I understand. {_generate_with_chatgpt("Generate a sentence to say it's time to end the talk by continuing the conversation in 50 words. ")}  Thank you for your time.</t>
+    <t>confirmation_request="Sorry to ask you again, but do you often eat sadwiches?"</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>topic_sandwich=#favorite-sandwich</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>confirmed=="yes"</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>confirmed=="no"</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>#favorite-sandwich=="egg salad sandwich"</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>I understand. {$"Generate a sentence to say it's time to end the talk by continuing the conversation in 50 words" }  Thank you for your time.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>$"Please determine if the user said the reason."</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -940,8 +942,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC9D1DC6-E066-4D71-9ECD-01107058A46B}">
   <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -988,10 +990,10 @@
         <v>28</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H2" s="9" t="s">
         <v>42</v>
@@ -1005,19 +1007,19 @@
         <v>42</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.4">
@@ -1028,7 +1030,7 @@
         <v>42</v>
       </c>
       <c r="H4" s="10" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="8" customFormat="1" ht="56.25" x14ac:dyDescent="0.4">
@@ -1036,10 +1038,10 @@
         <v>28</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>9</v>
@@ -1056,7 +1058,7 @@
         <v>28</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>8</v>
@@ -1073,16 +1075,16 @@
         <v>28</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>62</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="15" customFormat="1" ht="56.25" x14ac:dyDescent="0.4">
@@ -1090,10 +1092,10 @@
         <v>28</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D8" s="15" t="s">
         <v>9</v>
@@ -1110,7 +1112,7 @@
         <v>28</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D9" s="15" t="s">
         <v>8</v>
@@ -1127,16 +1129,16 @@
         <v>28</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D10" s="15" t="s">
         <v>62</v>
       </c>
       <c r="G10" s="15" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="H10" s="15" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.4">
@@ -1144,14 +1146,14 @@
         <v>28</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D11" s="8"/>
       <c r="F11" s="7" t="s">
-        <v>87</v>
+        <v>104</v>
       </c>
       <c r="G11" s="8"/>
       <c r="H11" s="8" t="s">
@@ -1163,12 +1165,12 @@
         <v>28</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
       <c r="F12" s="7" t="s">
-        <v>88</v>
+        <v>105</v>
       </c>
       <c r="G12" s="8"/>
       <c r="H12" s="12" t="s">
@@ -1223,7 +1225,7 @@
         <v>19</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="H15" s="12" t="s">
         <v>43</v>
@@ -1237,7 +1239,7 @@
         <v>12</v>
       </c>
       <c r="H16" s="12" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="17" spans="1:8" s="13" customFormat="1" ht="37.5" x14ac:dyDescent="0.4">
@@ -1257,13 +1259,13 @@
         <v>21</v>
       </c>
       <c r="F17" s="13" t="s">
-        <v>64</v>
+        <v>106</v>
       </c>
       <c r="G17" s="13" t="s">
-        <v>80</v>
+        <v>103</v>
       </c>
       <c r="H17" s="13" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18" spans="1:8" s="13" customFormat="1" ht="37.5" x14ac:dyDescent="0.4">
@@ -1280,13 +1282,13 @@
         <v>21</v>
       </c>
       <c r="F18" s="13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G18" s="13" t="s">
-        <v>66</v>
+        <v>103</v>
       </c>
       <c r="H18" s="13" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19" spans="1:8" s="13" customFormat="1" ht="37.5" x14ac:dyDescent="0.4">
@@ -1303,7 +1305,7 @@
         <v>21</v>
       </c>
       <c r="F19" s="13" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H19" s="13" t="s">
         <v>23</v>
@@ -1334,7 +1336,7 @@
         <v>60</v>
       </c>
       <c r="G21" s="9" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="H21" s="9" t="s">
         <v>43</v>
@@ -1345,7 +1347,7 @@
         <v>28</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C22" s="10" t="s">
         <v>56</v>
@@ -1354,7 +1356,7 @@
         <v>47</v>
       </c>
       <c r="G22" s="10" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="H22" s="10" t="s">
         <v>43</v>
@@ -1365,7 +1367,7 @@
         <v>28</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C23" s="8" t="s">
         <v>57</v>
@@ -1374,13 +1376,13 @@
         <v>24</v>
       </c>
       <c r="G23" s="8" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="H23" s="8" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" s="14" customFormat="1" ht="93.75" x14ac:dyDescent="0.4">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" s="14" customFormat="1" ht="75" x14ac:dyDescent="0.4">
       <c r="A24" s="14" t="s">
         <v>28</v>
       </c>
@@ -1388,7 +1390,7 @@
         <v>43</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="25" spans="1:8" s="14" customFormat="1" ht="37.5" x14ac:dyDescent="0.4">
@@ -1396,10 +1398,10 @@
         <v>28</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>43</v>
+        <v>100</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
     </row>
     <row r="26" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.4">
@@ -1407,10 +1409,10 @@
         <v>28</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="27" spans="1:8" s="10" customFormat="1" ht="37.5" x14ac:dyDescent="0.4">
@@ -1418,10 +1420,10 @@
         <v>28</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="28" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.4">
@@ -1440,20 +1442,20 @@
         <v>28</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D29" s="10"/>
       <c r="E29" s="6" t="s">
         <v>6</v>
       </c>
       <c r="G29" s="10" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="H29" s="6" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="30" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.4">
@@ -1461,15 +1463,15 @@
         <v>28</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C30" s="10"/>
       <c r="D30" s="10"/>
       <c r="G30" s="10" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="H30" s="6" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1505,7 +1507,7 @@
         <v>4</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.4">
@@ -1538,10 +1540,10 @@
         <v>27</v>
       </c>
       <c r="C4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.4">
@@ -1552,10 +1554,10 @@
         <v>27</v>
       </c>
       <c r="C5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.4">
@@ -1569,7 +1571,7 @@
         <v>61</v>
       </c>
       <c r="D6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.4">
@@ -1632,7 +1634,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>5</v>
@@ -1643,7 +1645,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B2" t="s">
         <v>63</v>
@@ -1657,7 +1659,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>32</v>
@@ -1668,7 +1670,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>41</v>
@@ -1677,7 +1679,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>34</v>
@@ -1686,7 +1688,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>35</v>
@@ -1695,7 +1697,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>36</v>
@@ -1704,7 +1706,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>37</v>
@@ -1713,7 +1715,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>38</v>
@@ -1722,7 +1724,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>39</v>
@@ -1731,7 +1733,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>40</v>

</xml_diff>

<commit_message>
docs updated for v0.8
</commit_message>
<xml_diff>
--- a/sample_apps/lab_app_en/lab_app_en_knowledge.xlsx
+++ b/sample_apps/lab_app_en/lab_app_en_knowledge.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nakano\system\dialbb\dialbb-next\sample_apps\lab_app_en\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B134791A-C885-4F52-9F49-8F5969BCE7C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50A59C1F-3EB5-4F4F-9DBD-2D337A958FA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{C3566FB2-A815-41D8-9347-99D11DD601B4}"/>
   </bookViews>
@@ -415,14 +415,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>_set(&amp;user_name, #NE_PERSON)</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>_ne(#NE_PERSON, "")</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>{greeting}. I'm {get_system_name()}. If you don't mind, could you tell me your name?</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -460,6 +452,14 @@
   </si>
   <si>
     <t>$"Please determine if the user said the reason."</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>user_name=#NE_PERSON</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>#NE_PERSON!=""</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -942,8 +942,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC9D1DC6-E066-4D71-9ECD-01107058A46B}">
   <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -1007,16 +1007,16 @@
         <v>42</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>78</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="H3" s="10" t="s">
         <v>79</v>
@@ -1081,7 +1081,7 @@
         <v>62</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H7" s="8" t="s">
         <v>89</v>
@@ -1153,7 +1153,7 @@
       </c>
       <c r="D11" s="8"/>
       <c r="F11" s="7" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G11" s="8"/>
       <c r="H11" s="8" t="s">
@@ -1170,7 +1170,7 @@
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
       <c r="F12" s="7" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G12" s="8"/>
       <c r="H12" s="12" t="s">
@@ -1225,7 +1225,7 @@
         <v>19</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H15" s="12" t="s">
         <v>43</v>
@@ -1239,7 +1239,7 @@
         <v>12</v>
       </c>
       <c r="H16" s="12" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="17" spans="1:8" s="13" customFormat="1" ht="37.5" x14ac:dyDescent="0.4">
@@ -1259,10 +1259,10 @@
         <v>21</v>
       </c>
       <c r="F17" s="13" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G17" s="13" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H17" s="13" t="s">
         <v>66</v>
@@ -1285,7 +1285,7 @@
         <v>64</v>
       </c>
       <c r="G18" s="13" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H18" s="13" t="s">
         <v>67</v>
@@ -1390,7 +1390,7 @@
         <v>43</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="25" spans="1:8" s="14" customFormat="1" ht="37.5" x14ac:dyDescent="0.4">
@@ -1398,10 +1398,10 @@
         <v>28</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="26" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
fixed bug in lab app en knowledge
</commit_message>
<xml_diff>
--- a/sample_apps/lab_app_en/lab_app_en_knowledge.xlsx
+++ b/sample_apps/lab_app_en/lab_app_en_knowledge.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nakano\system\dialbb\dialbb-next\sample_apps\lab_app_en\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nakano\system\dialbb\dialbb-main\sample_apps\lab_app_en\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B511AECD-4644-4705-ABC1-47B146D15E22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{238F080C-727E-4B31-A8A4-8094F78103EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32520" yWindow="2655" windowWidth="21600" windowHeight="11505" activeTab="2" xr2:uid="{C3566FB2-A815-41D8-9347-99D11DD601B4}"/>
+    <workbookView xWindow="35595" yWindow="2655" windowWidth="21540" windowHeight="11265" activeTab="2" xr2:uid="{C3566FB2-A815-41D8-9347-99D11DD601B4}"/>
   </bookViews>
   <sheets>
     <sheet name="scenario" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="117">
   <si>
     <t>conditions</t>
     <phoneticPr fontId="1"/>
@@ -493,10 +493,6 @@
   </si>
   <si>
     <t>Vegetable Sandwiches, vegetable</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>cd s</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -504,18 +500,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="6"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -523,7 +519,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -983,20 +979,20 @@
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.625" style="11"/>
+    <col min="1" max="1" width="8.5703125" style="11"/>
     <col min="2" max="2" width="28" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.5" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.875" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.5" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="35.625" style="11" customWidth="1"/>
-    <col min="7" max="7" width="40.25" style="11" customWidth="1"/>
-    <col min="8" max="8" width="46.375" style="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.625" style="11"/>
+    <col min="3" max="3" width="36.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.5703125" style="11" customWidth="1"/>
+    <col min="7" max="7" width="40.28515625" style="11" customWidth="1"/>
+    <col min="8" max="8" width="46.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.5703125" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:8" s="8" customFormat="1" ht="30">
       <c r="A1" s="8" t="s">
         <v>3</v>
       </c>
@@ -1022,7 +1018,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:8" s="9" customFormat="1">
       <c r="A2" s="9" t="s">
         <v>28</v>
       </c>
@@ -1036,7 +1032,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="10" customFormat="1" ht="56.25" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:8" s="10" customFormat="1" ht="45">
       <c r="A3" s="10" t="s">
         <v>28</v>
       </c>
@@ -1059,7 +1055,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:8" s="10" customFormat="1">
       <c r="A4" s="10" t="s">
         <v>28</v>
       </c>
@@ -1070,7 +1066,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="8" customFormat="1" ht="56.25" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:8" s="8" customFormat="1" ht="45">
       <c r="A5" s="8" t="s">
         <v>28</v>
       </c>
@@ -1090,7 +1086,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:8" s="8" customFormat="1">
       <c r="A6" s="8" t="s">
         <v>28</v>
       </c>
@@ -1107,7 +1103,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="8" customFormat="1" ht="37.5" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:8" s="8" customFormat="1" ht="30">
       <c r="A7" s="8" t="s">
         <v>28</v>
       </c>
@@ -1124,7 +1120,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="15" customFormat="1" ht="56.25" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:8" s="15" customFormat="1" ht="45">
       <c r="A8" s="15" t="s">
         <v>28</v>
       </c>
@@ -1144,7 +1140,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:8" s="15" customFormat="1">
       <c r="A9" s="15" t="s">
         <v>28</v>
       </c>
@@ -1161,7 +1157,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="15" customFormat="1" ht="37.5" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:8" s="15" customFormat="1" ht="45">
       <c r="A10" s="15" t="s">
         <v>28</v>
       </c>
@@ -1178,7 +1174,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:8" s="7" customFormat="1">
       <c r="A11" s="7" t="s">
         <v>28</v>
       </c>
@@ -1197,7 +1193,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:8" s="7" customFormat="1">
       <c r="A12" s="7" t="s">
         <v>28</v>
       </c>
@@ -1214,7 +1210,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:8" s="10" customFormat="1">
       <c r="A13" s="10" t="s">
         <v>28</v>
       </c>
@@ -1234,7 +1230,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:8" s="10" customFormat="1">
       <c r="A14" s="10" t="s">
         <v>28</v>
       </c>
@@ -1248,7 +1244,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:8" s="12" customFormat="1" ht="37.5" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:8" s="12" customFormat="1" ht="30">
       <c r="A15" s="12" t="s">
         <v>28</v>
       </c>
@@ -1268,7 +1264,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:8" s="12" customFormat="1">
       <c r="A16" s="12" t="s">
         <v>28</v>
       </c>
@@ -1279,7 +1275,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="17" spans="1:8" s="13" customFormat="1" ht="37.5" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:8" s="13" customFormat="1" ht="30">
       <c r="A17" s="13" t="s">
         <v>28</v>
       </c>
@@ -1305,7 +1301,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="1:8" s="13" customFormat="1" ht="37.5" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:8" s="13" customFormat="1" ht="30">
       <c r="A18" s="13" t="s">
         <v>28</v>
       </c>
@@ -1328,7 +1324,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="19" spans="1:8" s="13" customFormat="1" ht="37.5" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:8" s="13" customFormat="1" ht="30">
       <c r="A19" s="13" t="s">
         <v>28</v>
       </c>
@@ -1348,7 +1344,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:8" s="13" customFormat="1" ht="37.5" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:8" s="13" customFormat="1" ht="30">
       <c r="A20" s="13" t="s">
         <v>28</v>
       </c>
@@ -1362,7 +1358,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="1:8" s="9" customFormat="1" ht="56.25" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:8" s="9" customFormat="1" ht="45">
       <c r="A21" s="9" t="s">
         <v>28</v>
       </c>
@@ -1379,7 +1375,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:8" s="10" customFormat="1" ht="37.5" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:8" s="10" customFormat="1" ht="45">
       <c r="A22" s="10" t="s">
         <v>28</v>
       </c>
@@ -1399,7 +1395,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:8" s="8" customFormat="1" ht="37.5" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:8" s="8" customFormat="1" ht="30">
       <c r="A23" s="8" t="s">
         <v>28</v>
       </c>
@@ -1419,7 +1415,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="24" spans="1:8" s="14" customFormat="1" ht="75" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:8" s="14" customFormat="1" ht="60">
       <c r="A24" s="14" t="s">
         <v>28</v>
       </c>
@@ -1430,7 +1426,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="25" spans="1:8" s="14" customFormat="1" ht="37.5" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:8" s="14" customFormat="1" ht="30">
       <c r="A25" s="14" t="s">
         <v>28</v>
       </c>
@@ -1441,7 +1437,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="26" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:8" s="10" customFormat="1">
       <c r="A26" s="10" t="s">
         <v>28</v>
       </c>
@@ -1452,7 +1448,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="27" spans="1:8" s="10" customFormat="1" ht="37.5" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:8" s="10" customFormat="1" ht="30">
       <c r="A27" s="10" t="s">
         <v>28</v>
       </c>
@@ -1463,7 +1459,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="28" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:8" s="9" customFormat="1">
       <c r="A28" s="9" t="s">
         <v>28</v>
       </c>
@@ -1474,7 +1470,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="29" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:8" s="6" customFormat="1">
       <c r="A29" s="6" t="s">
         <v>28</v>
       </c>
@@ -1495,7 +1491,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="30" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:8" s="6" customFormat="1">
       <c r="A30" s="6" t="s">
         <v>28</v>
       </c>
@@ -1526,14 +1522,14 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="61.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="41.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="61.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -1547,7 +1543,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -1558,7 +1554,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -1569,7 +1565,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -1583,7 +1579,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>28</v>
       </c>
@@ -1597,7 +1593,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -1611,7 +1607,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -1622,7 +1618,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -1633,7 +1629,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>28</v>
       </c>
@@ -1656,17 +1652,17 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="17.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="53" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1680,12 +1676,12 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>70</v>
       </c>
       <c r="B2" t="s">
-        <v>117</v>
+        <v>62</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>30</v>
@@ -1694,7 +1690,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>70</v>
       </c>
@@ -1708,7 +1704,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>70</v>
       </c>
@@ -1722,7 +1718,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>70</v>
       </c>
@@ -1736,7 +1732,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>70</v>
       </c>
@@ -1750,7 +1746,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>70</v>
       </c>
@@ -1764,7 +1760,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>70</v>
       </c>
@@ -1778,7 +1774,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>70</v>
       </c>
@@ -1792,7 +1788,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>70</v>
       </c>
@@ -1806,7 +1802,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>70</v>
       </c>

</xml_diff>